<commit_message>
V2I2 regenerated output files, design in progress
</commit_message>
<xml_diff>
--- a/EPS-LKAS/V2I1/Project Outputs for MCU_EPS/BOM/Bill of Materials-EPS-LKAS Manipulator.xlsx
+++ b/EPS-LKAS/V2I1/Project Outputs for MCU_EPS/BOM/Bill of Materials-EPS-LKAS Manipulator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mloco\Google Drive\Design\Altium Design Files\Design Files\serialSteeringHardware\EPS-LKAS\V1I1\Project Outputs for MCU_EPS\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mloco\Google Drive\Design\Altium Design Files\Design Files\serialSteeringHardware\EPS-LKAS\V2I1\Project Outputs for MCU_EPS\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CD32639-B1E8-42B6-ADB2-E32E1DDFF2CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72AE2997-CE92-48EC-97FC-60954B29E4B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="19200" windowHeight="10060" xr2:uid="{4A6A6350-80F9-4F84-9610-7390E5DED720}"/>
+    <workbookView xWindow="4030" yWindow="4040" windowWidth="19200" windowHeight="10060" xr2:uid="{C05DF2FF-3E03-406F-A822-A93C8F30E640}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-EPS-LKAS Mani" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>Comment</t>
   </si>
@@ -57,31 +57,34 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Teensy 4.0</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>BRD1</t>
-  </si>
-  <si>
-    <t>tEENSY 4.0</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 100V X7R 0805</t>
-  </si>
-  <si>
-    <t>C1, C3, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14</t>
-  </si>
-  <si>
-    <t>C0805</t>
-  </si>
-  <si>
-    <t>CL21B104KCFWPNE</t>
+    <t>C0603C104M3RACTU</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>C1, C2, C8, C9, C10, C11, C12, C13, C14, C15</t>
+  </si>
+  <si>
+    <t>FP-C0603C-CF-MFG</t>
+  </si>
+  <si>
+    <t>CMP-2006-03065-2</t>
+  </si>
+  <si>
+    <t>CL10B475KQ8NQNC</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 6.3V X7R 0603</t>
+  </si>
+  <si>
+    <t>C3, C7, C16</t>
+  </si>
+  <si>
+    <t>FP-CL10-IPC_C</t>
+  </si>
+  <si>
+    <t>CMP-2000-06096-2</t>
   </si>
   <si>
     <t>CL31A106KBHNNNE</t>
@@ -99,6 +102,21 @@
     <t>CMP-13271-000016-1</t>
   </si>
   <si>
+    <t>GRM1885C1H220JA01D</t>
+  </si>
+  <si>
+    <t>Chip Capacitor, 22 pF, +/- 5%, 50 V, -55 to 125 degC, 0603 (1608 Metric), RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>C5, C6</t>
+  </si>
+  <si>
+    <t>CAPC1608X90X35ML10T15</t>
+  </si>
+  <si>
+    <t>CMP-2000-04945-1</t>
+  </si>
+  <si>
     <t>1812L050/30PR</t>
   </si>
   <si>
@@ -132,18 +150,6 @@
     <t>J2</t>
   </si>
   <si>
-    <t>686115148922</t>
-  </si>
-  <si>
-    <t>SMT ZIF Connectors Hinge Type WR-FPC, Horizontal, Bottom Contact, pitch 1 mm, 15 pins</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>CMP-1502-01518-1</t>
-  </si>
-  <si>
     <t>150080SS75000</t>
   </si>
   <si>
@@ -171,43 +177,58 @@
     <t>CMP-1426-00008-1</t>
   </si>
   <si>
-    <t>4K7 1%</t>
-  </si>
-  <si>
-    <t>4K7 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8, R22, R23</t>
-  </si>
-  <si>
-    <t>RESC0603(1608)_N</t>
-  </si>
-  <si>
-    <t>CMP-1012-00586-1</t>
-  </si>
-  <si>
-    <t>CRCW0805330RFKEA</t>
-  </si>
-  <si>
-    <t>R14, R17</t>
-  </si>
-  <si>
-    <t>RESC2013X50X30NL20T20</t>
-  </si>
-  <si>
-    <t>CMP-2001-03823-1</t>
-  </si>
-  <si>
-    <t>76STC04T</t>
+    <t>62201421121</t>
+  </si>
+  <si>
+    <t>THT Vertical Pin Header WR-PHD, Pitch 1.27 mm, Dual Row, 14 pins</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>CMP-1502-00949-1</t>
+  </si>
+  <si>
+    <t>4K7</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0603 4.7K Ohm 1% 1/10W 100ppm/C Molded SMD SMD Paper T/R</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R11, R12, R22, R23</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT4K70</t>
+  </si>
+  <si>
+    <t>RC0603FR-07560RL</t>
+  </si>
+  <si>
+    <t>Chip Resistor, 560 Ohm, +/- 1%, 0.1 W, -55 to 155 degC, 0603 (1608 Metric), RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>R9, R10</t>
+  </si>
+  <si>
+    <t>RESC1608X55X25ML10T15</t>
+  </si>
+  <si>
+    <t>CMP-1659-00038-1</t>
+  </si>
+  <si>
+    <t>76STC02T</t>
   </si>
   <si>
     <t>SWITCH TOGGLE DIP SPDT 150MA 30V_x000D_
 WIRED:_x000D_
-1  2  3  4   5   6_x000D_
-7  8  9  10 11 12</t>
-  </si>
-  <si>
-    <t>SW6</t>
+1  2  3_x000D_
+4  5  6</t>
+  </si>
+  <si>
+    <t>SW1</t>
   </si>
   <si>
     <t>UA7805CKTTR</t>
@@ -232,12 +253,27 @@
     <t>8 SOIC 3.90mm(.150in) TUBECAN Flexible Data Rate Transceiver</t>
   </si>
   <si>
-    <t>U2, U3</t>
+    <t>U2</t>
   </si>
   <si>
     <t>MCP2561</t>
   </si>
   <si>
+    <t>MIC5504-3.3YM5-TR</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 300MA SOT23-5</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>FP-SOT23-5LD-PL-1-MFG</t>
+  </si>
+  <si>
+    <t>CMP-2000-07604-2</t>
+  </si>
+  <si>
     <t>LM339DR2G</t>
   </si>
   <si>
@@ -251,6 +287,36 @@
   </si>
   <si>
     <t>CMP-1305-00036-1</t>
+  </si>
+  <si>
+    <t>STM32F103T6U6A</t>
+  </si>
+  <si>
+    <t>ARM Cortex-M3 32-bit MCU, 32 KB Flash, 10 KB Internal RAM, 26 I/Os, 36-pin VFQFPN, -40 to 85 degC, Tray</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>STM-VFQFPN36_N</t>
+  </si>
+  <si>
+    <t>CMP-0237-00043-3</t>
+  </si>
+  <si>
+    <t>ABM7-8.000MHZ-D2Y-T</t>
+  </si>
+  <si>
+    <t>Microprocessor Crystal, 8 MHz, 18 PF, -40 to 85 degC, 2-Pin SMD, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>ABRA-ABM7-2_V</t>
+  </si>
+  <si>
+    <t>CMP-2000-05034-1</t>
   </si>
 </sst>
 </file>
@@ -632,11 +698,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903DE72E-11BF-449A-A7A8-1B0FD0C454C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC73DD4-9292-4ED3-906E-6366EA048F10}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -665,7 +731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -679,107 +745,107 @@
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="4">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -787,16 +853,16 @@
     </row>
     <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>34</v>
@@ -807,19 +873,19 @@
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -827,96 +893,96 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F11" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F12" s="4">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>60</v>
@@ -925,49 +991,129 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F15" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="F16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="69" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="49" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated to use STM32F1 48 pin package. Added USB programming Port, added OR for 3.3V input
</commit_message>
<xml_diff>
--- a/EPS-LKAS/V2I1/Project Outputs for MCU_EPS/BOM/Bill of Materials-EPS-LKAS Manipulator.xlsx
+++ b/EPS-LKAS/V2I1/Project Outputs for MCU_EPS/BOM/Bill of Materials-EPS-LKAS Manipulator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mloco\Google Drive\Design\Altium Design Files\Design Files\serialSteeringHardware\EPS-LKAS\V2I1\Project Outputs for MCU_EPS\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72AE2997-CE92-48EC-97FC-60954B29E4B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4CC2C4-AD8F-49F5-9798-E31FF027F817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4030" yWindow="4040" windowWidth="19200" windowHeight="10060" xr2:uid="{C05DF2FF-3E03-406F-A822-A93C8F30E640}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{A1208D70-8513-498E-9A5F-EC33FF32C5B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-EPS-LKAS Mani" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="109">
   <si>
     <t>Comment</t>
   </si>
@@ -117,6 +117,21 @@
     <t>CMP-2000-04945-1</t>
   </si>
   <si>
+    <t>SS14</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 1A SMA</t>
+  </si>
+  <si>
+    <t>D1, D2</t>
+  </si>
+  <si>
+    <t>FP-403AE-MFG</t>
+  </si>
+  <si>
+    <t>CMP-2000-04943-2</t>
+  </si>
+  <si>
     <t>1812L050/30PR</t>
   </si>
   <si>
@@ -150,6 +165,21 @@
     <t>J2</t>
   </si>
   <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>Micro USB B Type Receptacle, -55 to 85 degC, 5-Pin SMD, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>FCI-10118192-0001LF-5_V</t>
+  </si>
+  <si>
+    <t>CMP-2000-05118-1</t>
+  </si>
+  <si>
     <t>150080SS75000</t>
   </si>
   <si>
@@ -177,25 +207,13 @@
     <t>CMP-1426-00008-1</t>
   </si>
   <si>
-    <t>62201421121</t>
-  </si>
-  <si>
-    <t>THT Vertical Pin Header WR-PHD, Pitch 1.27 mm, Dual Row, 14 pins</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>CMP-1502-00949-1</t>
-  </si>
-  <si>
     <t>4K7</t>
   </si>
   <si>
     <t>Res Thick Film 0603 4.7K Ohm 1% 1/10W 100ppm/C Molded SMD SMD Paper T/R</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8, R11, R12, R22, R23</t>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R11, R12, R13, R22, R23</t>
   </si>
   <si>
     <t>R0603</t>
@@ -217,6 +235,21 @@
   </si>
   <si>
     <t>CMP-1659-00038-1</t>
+  </si>
+  <si>
+    <t>CRCW060322R0JNTA</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>R14, R15</t>
+  </si>
+  <si>
+    <t>RESC1609X50X30ML10T20</t>
+  </si>
+  <si>
+    <t>CMP-2000-03099-1</t>
   </si>
   <si>
     <t>76STC02T</t>
@@ -289,19 +322,34 @@
     <t>CMP-1305-00036-1</t>
   </si>
   <si>
-    <t>STM32F103T6U6A</t>
-  </si>
-  <si>
-    <t>ARM Cortex-M3 32-bit MCU, 32 KB Flash, 10 KB Internal RAM, 26 I/Os, 36-pin VFQFPN, -40 to 85 degC, Tray</t>
+    <t>STM32F103C6T7ATR</t>
+  </si>
+  <si>
+    <t>ARM Cortex-M3 32-bit MCU, 32 KB Flash, 10 KB Internal RAM, 37 I/Os, 48-pin LQFP, -40 to 105 degC, Tape and Reel</t>
   </si>
   <si>
     <t>U5</t>
   </si>
   <si>
-    <t>STM-VFQFPN36_N</t>
-  </si>
-  <si>
-    <t>CMP-0237-00043-3</t>
+    <t>STM-LQFP48_L</t>
+  </si>
+  <si>
+    <t>CMP-0237-00257-3</t>
+  </si>
+  <si>
+    <t>STM32F103C6U6A</t>
+  </si>
+  <si>
+    <t>ARM Cortex-M3 32-bit MCU, 32 KB Flash, 10 KB Internal RAM, 37 I/Os, 48-pin UFQFPN, -40 to 85 degC, Tray</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>STM-UFQFPN48_M</t>
+  </si>
+  <si>
+    <t>CMP-0237-00046-3</t>
   </si>
   <si>
     <t>ABM7-8.000MHZ-D2Y-T</t>
@@ -317,6 +365,9 @@
   </si>
   <si>
     <t>CMP-2000-05034-1</t>
+  </si>
+  <si>
+    <t>PREFERRED* OVER U6</t>
   </si>
 </sst>
 </file>
@@ -346,7 +397,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -369,11 +420,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -383,6 +445,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -698,17 +763,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC73DD4-9292-4ED3-906E-6366EA048F10}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD9500C-2A4E-43F6-9AB7-6DC62AEA4E54}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -811,7 +879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -828,10 +896,10 @@
         <v>30</v>
       </c>
       <c r="F6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -842,56 +910,56 @@
         <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -902,218 +970,281 @@
         <v>44</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F12" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F13" s="4">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="49" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="43" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated, cleaned files and regenerated gerber after last modification
</commit_message>
<xml_diff>
--- a/EPS-LKAS/V2I1/Project Outputs for MCU_EPS/BOM/Bill of Materials-EPS-LKAS Manipulator.xlsx
+++ b/EPS-LKAS/V2I1/Project Outputs for MCU_EPS/BOM/Bill of Materials-EPS-LKAS Manipulator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mloco\Google Drive\Design\Altium Design Files\Design Files\serialSteeringHardware\EPS-LKAS\V2I1\Project Outputs for MCU_EPS\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4CC2C4-AD8F-49F5-9798-E31FF027F817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE683B0-9443-461A-A322-869E424C2941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{A1208D70-8513-498E-9A5F-EC33FF32C5B3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{EB428808-36ED-411D-88E4-569359AFC374}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-EPS-LKAS Mani" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="113">
   <si>
     <t>Comment</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>CRCW060322R0JNTA</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>R14, R15</t>
@@ -307,12 +304,6 @@
     <t>CMP-2000-07604-2</t>
   </si>
   <si>
-    <t>LM339DR2G</t>
-  </si>
-  <si>
-    <t>Single Supply Quad Comparators, 0 to 70 degC, 14-Pin SOIC, Pb-Free, Tape and Reel</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -367,7 +358,28 @@
     <t>CMP-2000-05034-1</t>
   </si>
   <si>
-    <t>PREFERRED* OVER U6</t>
+    <t>Select U5 or equivalent for LQFP48 footprint</t>
+  </si>
+  <si>
+    <t>Select U6 or quivalent for UFQFPN48 footprint</t>
+  </si>
+  <si>
+    <t>1 or U5</t>
+  </si>
+  <si>
+    <t>1 or u6</t>
+  </si>
+  <si>
+    <t>NCV2901DR2G</t>
+  </si>
+  <si>
+    <t>Comparator General Purpose CMOS, Open-Collector, TTL 14-SOIC</t>
+  </si>
+  <si>
+    <t>22R 0603</t>
+  </si>
+  <si>
+    <t>Note, pins are needed - no PCB equivalent exists.</t>
   </si>
 </sst>
 </file>
@@ -397,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -431,11 +443,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -449,6 +470,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,23 +787,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD9500C-2A4E-43F6-9AB7-6DC62AEA4E54}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFDF7F0E-EA53-4CC6-9789-296A8BBBD90C}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="6" width="18.81640625" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -799,7 +823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -819,7 +843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -839,7 +863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -859,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -879,7 +903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -899,7 +923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -919,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
@@ -938,8 +962,11 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="G8" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -959,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -979,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
@@ -999,7 +1026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1019,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>56</v>
       </c>
@@ -1039,7 +1066,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>61</v>
       </c>
@@ -1059,190 +1086,198 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="F21" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="4">
-        <v>1</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="F22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="F23" s="4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H21:H22"/>
+  </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
   <pageSetup scale="43" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>